<commit_message>
fix bugs and add some features
</commit_message>
<xml_diff>
--- a/schedule/history/2022年1月值班安排.xlsx
+++ b/schedule/history/2022年1月值班安排.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,27 +429,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>星期几</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>值班人员</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>星期</t>
-        </is>
-      </c>
       <c r="D1" t="inlineStr">
         <is>
           <t>是否节假日</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>最后工作日系数</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>节假日系数</t>
         </is>
       </c>
     </row>
@@ -461,22 +451,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>周六</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>苹果</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>6</v>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -487,22 +473,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>周天</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>梨子</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>7</v>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -513,22 +495,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>苹果</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
+          <t>周一</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>山竹</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
+          <t>Y</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -539,22 +517,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>梨子</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
+          <t>周二</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>苹果</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -565,22 +539,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>山竹</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>3</v>
+          <t>周三</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>梨子</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -591,22 +561,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>西瓜</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>4</v>
+          <t>周四</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>山竹</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -617,22 +583,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>菠萝</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>5</v>
+          <t>周五</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>串串香</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -643,22 +605,18 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>山竹</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>6</v>
+          <t>周六</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>樱桃</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -669,22 +627,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>西瓜</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>7</v>
+          <t>周天</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>桔子</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -695,22 +649,18 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>甘蔗</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
+          <t>周一</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>西瓜</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -721,22 +671,18 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>桔子</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>2</v>
+          <t>周二</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>香蕉</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -747,22 +693,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>芒果</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>3</v>
+          <t>周三</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>菠萝</t>
+        </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -773,22 +715,18 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>榴莲</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>4</v>
+          <t>周四</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>甘蔗</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -799,22 +737,18 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>烤鱼</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>5</v>
+          <t>周五</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>樱桃</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -825,22 +759,18 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>菠萝</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>6</v>
+          <t>周六</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>香蕉</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -851,22 +781,18 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>甘蔗</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>7</v>
+          <t>周天</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>西瓜</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -877,22 +803,18 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>串串香</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
+          <t>周一</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>芒果</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -903,22 +825,18 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>烤羊排</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>2</v>
+          <t>周二</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>榴莲</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -929,22 +847,18 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>苹果</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>3</v>
+          <t>周三</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>炸排骨</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -955,22 +869,18 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>梨子</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>4</v>
+          <t>周四</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>烤鱼</t>
+        </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -981,22 +891,18 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>山竹</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>5</v>
+          <t>周五</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>桔子</t>
+        </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1007,22 +913,18 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>桔子</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>6</v>
+          <t>周六</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>甘蔗</t>
+        </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1033,22 +935,18 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>芒果</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>7</v>
+          <t>周天</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>菠萝</t>
+        </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1059,22 +957,18 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>西瓜</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
+          <t>周一</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>烤羊排</t>
+        </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1085,22 +979,18 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>菠萝</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>2</v>
+          <t>周二</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>苹果</t>
+        </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1111,22 +1001,18 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>甘蔗</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>3</v>
+          <t>周三</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>梨子</t>
+        </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1137,22 +1023,18 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>桔子</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>4</v>
+          <t>周四</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>山竹</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1163,22 +1045,18 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>芒果</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>5</v>
+          <t>周五</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>樱桃</t>
+        </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>N</t>
         </is>
-      </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1189,22 +1067,18 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>榴莲</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>6</v>
+          <t>周六</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>西瓜</t>
+        </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1215,22 +1089,18 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>烤鱼</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>7</v>
+          <t>周天</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>香蕉</t>
+        </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1241,22 +1111,18 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>榴莲</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>1</v>
+          <t>周一</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>芒果</t>
+        </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0</v>
+          <t>Y</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>